<commit_message>
prese 10 misurazioni con sferette di diametri diversi (distanza di 20 cm)
</commit_message>
<xml_diff>
--- a/VISCOSITA/viscosità.xlsx
+++ b/VISCOSITA/viscosità.xlsx
@@ -4385,85 +4385,184 @@
       <c r="B1">
         <v>3</v>
       </c>
+      <c r="C1">
+        <v>4</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" s="9">
         <v>21.789999999999999</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>10.130000000000001</v>
       </c>
+      <c r="C3" s="9">
+        <v>6</v>
+      </c>
+      <c r="D3" s="9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E3" s="9">
+        <v>2.96</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="9">
         <v>21.5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="9">
         <v>10.300000000000001</v>
       </c>
+      <c r="C4" s="9">
+        <v>6.0199999999999996</v>
+      </c>
+      <c r="D4" s="9">
+        <v>4.0800000000000001</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2.96</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="9">
         <v>21.75</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <v>10.17</v>
       </c>
+      <c r="C5" s="9">
+        <v>6.0700000000000003</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4.04</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2.96</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="9">
         <v>22.039999999999999</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <v>10.24</v>
       </c>
+      <c r="C6" s="9">
+        <v>5.9100000000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>3.98</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2.9500000000000002</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="9">
         <v>21.710000000000001</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <v>10.19</v>
       </c>
+      <c r="C7" s="9">
+        <v>6.0700000000000003</v>
+      </c>
+      <c r="D7" s="9">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2.9500000000000002</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="9">
         <v>21.77</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <v>10.029999999999999</v>
       </c>
+      <c r="C8" s="9">
+        <v>6.0300000000000002</v>
+      </c>
+      <c r="D8" s="9">
+        <v>4.0700000000000003</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3.1299999999999999</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="9">
         <v>22.030000000000001</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <v>9.8100000000000005</v>
       </c>
+      <c r="C9" s="9">
+        <v>5.8399999999999999</v>
+      </c>
+      <c r="D9" s="9">
+        <v>3.98</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2.9100000000000001</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="9">
         <v>21.789999999999999</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="9">
         <v>9.8800000000000008</v>
       </c>
+      <c r="C10" s="9">
+        <v>5.8399999999999999</v>
+      </c>
+      <c r="D10" s="9">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.8300000000000001</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="9">
         <v>21.440000000000001</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="9">
         <v>10.029999999999999</v>
       </c>
+      <c r="C11" s="9">
+        <v>6.04</v>
+      </c>
+      <c r="D11" s="9">
+        <v>4.0099999999999998</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2.8900000000000001</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="9">
         <v>21.66</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>9.9399999999999995</v>
+      </c>
+      <c r="C12" s="9">
+        <v>5.8399999999999999</v>
+      </c>
+      <c r="D12" s="9">
+        <v>3.96</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2.9500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>